<commit_message>
Update spreadsheet with final state
</commit_message>
<xml_diff>
--- a/documentation/Matriz de transiciones de estados.xlsx
+++ b/documentation/Matriz de transiciones de estados.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="29">
   <si>
     <t>Simbolo/Estado</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>otro</t>
+  </si>
+  <si>
+    <t>$</t>
   </si>
 </sst>
 </file>
@@ -1764,24 +1767,60 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="P29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R29" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="5"/>

</xml_diff>